<commit_message>
Identificação dos casos de uso e Diagrama de UC
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8025"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
@@ -167,14 +167,71 @@
     <t>Emitir relatórios de despesas/receitas</t>
   </si>
   <si>
-    <t>Permitir que uma mesma despesa seja lançada em categorias diferentes</t>
+    <t>Permitir que o usuário altere seus dados</t>
+  </si>
+  <si>
+    <t>Registrar Usuário</t>
+  </si>
+  <si>
+    <t>Fazer Login</t>
+  </si>
+  <si>
+    <t>Recuperar Senha</t>
+  </si>
+  <si>
+    <t>Na primeira execução, permitir que o usuário escolha entre usar a lista de categorias padrão ou personalizada</t>
+  </si>
+  <si>
+    <t>Fazer configuração inicial</t>
+  </si>
+  <si>
+    <t>Manter categorias</t>
+  </si>
+  <si>
+    <t>Lançar movimentação</t>
+  </si>
+  <si>
+    <t>Registrar Fornecedor, Consultar Fornecedor</t>
+  </si>
+  <si>
+    <t>Manter Categorias</t>
+  </si>
+  <si>
+    <t>Manter Formas de Pagamento</t>
+  </si>
+  <si>
+    <t>Lançar Movimentação</t>
+  </si>
+  <si>
+    <t>Emitir Relatório</t>
+  </si>
+  <si>
+    <t>Permitir que uma despesa seja dividida em mais de uma categoria</t>
+  </si>
+  <si>
+    <t>Alterar Dados de Usuário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permitir que vários usuários usem o sistema em uma mesma máquina </t>
+  </si>
+  <si>
+    <t>Registrar Fornecedor</t>
+  </si>
+  <si>
+    <t>Consultar Fornecedor</t>
+  </si>
+  <si>
+    <t>UC11</t>
+  </si>
+  <si>
+    <t>Usuário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,21 +271,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -239,15 +324,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -266,18 +345,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,6 +458,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -399,6 +493,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -574,312 +669,405 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="C16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
+      <c r="B17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7" t="s">
+      <c r="B28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="7" t="s">
+      <c r="B29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7" t="s">
+      <c r="B30" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="7" t="s">
+      <c r="B31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="7" t="s">
+      <c r="B32" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="7" t="s">
+      <c r="B34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="7" t="s">
+      <c r="B35" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="7" t="s">
+      <c r="B36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="B40" s="5"/>
+      <c r="B37" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -893,12 +1081,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -910,12 +1098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Inclusão de Imagem do Diagrama de Casos de Uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8025"/>
@@ -342,7 +342,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -383,13 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -405,6 +399,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -453,7 +450,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,7 +485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,25 +900,25 @@
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>69</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="16" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="4"/>
@@ -1108,7 +1105,7 @@
       <c r="A39" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1119,7 +1116,7 @@
       <c r="A40" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C40" s="8" t="s">

</xml_diff>